<commit_message>
Added 6 new cases
</commit_message>
<xml_diff>
--- a/tools/ExporterSheet.xlsx
+++ b/tools/ExporterSheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7472" uniqueCount="1968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7552" uniqueCount="1992">
   <si>
     <t>NOUMBER</t>
   </si>
@@ -5915,6 +5915,78 @@
   </si>
   <si>
     <t>https://discord.gg/SpJqNPaB6Y</t>
+  </si>
+  <si>
+    <t>1143501896875782154</t>
+  </si>
+  <si>
+    <t>filip57.</t>
+  </si>
+  <si>
+    <t>https://steamshort.guru/s/LNMTK</t>
+  </si>
+  <si>
+    <t>291045824551452672</t>
+  </si>
+  <si>
+    <t>jordy3523</t>
+  </si>
+  <si>
+    <t>https://steanmecormmunity.com/105941095</t>
+  </si>
+  <si>
+    <t>1198324403298111689</t>
+  </si>
+  <si>
+    <t>ionut999996_75145</t>
+  </si>
+  <si>
+    <t>https://in.mt/fah</t>
+  </si>
+  <si>
+    <t>1199469959714197617</t>
+  </si>
+  <si>
+    <t>fthes_63529</t>
+  </si>
+  <si>
+    <t>https://in.mt/fsq</t>
+  </si>
+  <si>
+    <t>498079857578737685</t>
+  </si>
+  <si>
+    <t>azlayer90</t>
+  </si>
+  <si>
+    <t>https://u.to/3jMvIg</t>
+  </si>
+  <si>
+    <t>196963902527897600</t>
+  </si>
+  <si>
+    <t>krocokxd</t>
+  </si>
+  <si>
+    <t>https://u.to/z94DIg</t>
+  </si>
+  <si>
+    <t>734730620688662529</t>
+  </si>
+  <si>
+    <t>springtrap6033</t>
+  </si>
+  <si>
+    <t>https://is.gd/LlH1Pj</t>
+  </si>
+  <si>
+    <t>917516388103503912</t>
+  </si>
+  <si>
+    <t>etraxe</t>
+  </si>
+  <si>
+    <t>https://u.to/FyUvIg</t>
   </si>
 </sst>
 </file>
@@ -34583,108 +34655,308 @@
       </c>
     </row>
     <row r="748">
-      <c r="B748" s="2"/>
-      <c r="C748" s="3"/>
-      <c r="D748" s="1"/>
-      <c r="E748" s="1"/>
-      <c r="F748" s="1"/>
-      <c r="G748" s="1"/>
-      <c r="H748" s="1"/>
-      <c r="I748" s="1"/>
-      <c r="J748" s="1"/>
-      <c r="K748" s="1"/>
-      <c r="L748" s="1"/>
+      <c r="A748" s="1">
+        <v>747.0</v>
+      </c>
+      <c r="B748" s="2">
+        <v>45734.0</v>
+      </c>
+      <c r="C748" s="3" t="s">
+        <v>1968</v>
+      </c>
+      <c r="D748" s="1" t="s">
+        <v>1969</v>
+      </c>
+      <c r="E748" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F748" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G748" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H748" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I748" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J748" s="4" t="s">
+        <v>1970</v>
+      </c>
+      <c r="K748" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L748" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="749">
-      <c r="B749" s="2"/>
-      <c r="C749" s="3"/>
-      <c r="D749" s="1"/>
-      <c r="E749" s="1"/>
-      <c r="F749" s="1"/>
-      <c r="G749" s="1"/>
-      <c r="H749" s="1"/>
-      <c r="I749" s="1"/>
-      <c r="J749" s="1"/>
-      <c r="K749" s="1"/>
-      <c r="L749" s="1"/>
+      <c r="A749" s="1">
+        <v>748.0</v>
+      </c>
+      <c r="B749" s="2">
+        <v>45734.0</v>
+      </c>
+      <c r="C749" s="3" t="s">
+        <v>1971</v>
+      </c>
+      <c r="D749" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="E749" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F749" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G749" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H749" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I749" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J749" s="4" t="s">
+        <v>1973</v>
+      </c>
+      <c r="K749" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L749" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="750">
-      <c r="B750" s="2"/>
-      <c r="C750" s="3"/>
-      <c r="D750" s="1"/>
-      <c r="E750" s="1"/>
-      <c r="F750" s="1"/>
-      <c r="G750" s="1"/>
-      <c r="H750" s="1"/>
-      <c r="I750" s="1"/>
-      <c r="J750" s="1"/>
-      <c r="K750" s="1"/>
-      <c r="L750" s="1"/>
+      <c r="A750" s="1">
+        <v>749.0</v>
+      </c>
+      <c r="B750" s="2">
+        <v>45734.0</v>
+      </c>
+      <c r="C750" s="3" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D750" s="1" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E750" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F750" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G750" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H750" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I750" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J750" s="4" t="s">
+        <v>1976</v>
+      </c>
+      <c r="K750" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L750" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="751">
-      <c r="B751" s="2"/>
-      <c r="C751" s="3"/>
-      <c r="D751" s="1"/>
-      <c r="E751" s="1"/>
-      <c r="F751" s="1"/>
-      <c r="G751" s="1"/>
-      <c r="H751" s="1"/>
-      <c r="I751" s="1"/>
-      <c r="J751" s="1"/>
-      <c r="K751" s="1"/>
-      <c r="L751" s="1"/>
+      <c r="A751" s="1">
+        <v>750.0</v>
+      </c>
+      <c r="B751" s="2">
+        <v>45735.0</v>
+      </c>
+      <c r="C751" s="3" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D751" s="1" t="s">
+        <v>1978</v>
+      </c>
+      <c r="E751" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F751" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G751" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H751" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I751" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J751" s="4" t="s">
+        <v>1979</v>
+      </c>
+      <c r="K751" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L751" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="752">
-      <c r="B752" s="2"/>
-      <c r="C752" s="3"/>
-      <c r="D752" s="1"/>
-      <c r="E752" s="1"/>
-      <c r="F752" s="1"/>
-      <c r="G752" s="1"/>
-      <c r="H752" s="1"/>
-      <c r="I752" s="1"/>
-      <c r="J752" s="1"/>
-      <c r="K752" s="1"/>
-      <c r="L752" s="1"/>
+      <c r="A752" s="1">
+        <v>751.0</v>
+      </c>
+      <c r="B752" s="2">
+        <v>45736.0</v>
+      </c>
+      <c r="C752" s="3" t="s">
+        <v>1980</v>
+      </c>
+      <c r="D752" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="E752" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F752" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G752" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H752" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I752" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J752" s="4" t="s">
+        <v>1982</v>
+      </c>
+      <c r="K752" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L752" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="753">
-      <c r="B753" s="2"/>
-      <c r="C753" s="3"/>
-      <c r="D753" s="1"/>
-      <c r="E753" s="1"/>
-      <c r="F753" s="1"/>
-      <c r="G753" s="1"/>
-      <c r="H753" s="1"/>
-      <c r="I753" s="1"/>
-      <c r="J753" s="1"/>
-      <c r="K753" s="1"/>
-      <c r="L753" s="1"/>
+      <c r="A753" s="1">
+        <v>752.0</v>
+      </c>
+      <c r="B753" s="2">
+        <v>45741.0</v>
+      </c>
+      <c r="C753" s="3" t="s">
+        <v>1983</v>
+      </c>
+      <c r="D753" s="1" t="s">
+        <v>1984</v>
+      </c>
+      <c r="E753" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F753" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G753" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H753" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I753" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J753" s="4" t="s">
+        <v>1985</v>
+      </c>
+      <c r="K753" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L753" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="754">
-      <c r="B754" s="2"/>
-      <c r="C754" s="3"/>
-      <c r="D754" s="1"/>
-      <c r="E754" s="1"/>
-      <c r="F754" s="1"/>
-      <c r="G754" s="1"/>
-      <c r="H754" s="1"/>
-      <c r="I754" s="1"/>
-      <c r="J754" s="1"/>
-      <c r="K754" s="1"/>
-      <c r="L754" s="1"/>
+      <c r="A754" s="1">
+        <v>753.0</v>
+      </c>
+      <c r="B754" s="2">
+        <v>45711.0</v>
+      </c>
+      <c r="C754" s="3" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D754" s="1" t="s">
+        <v>1987</v>
+      </c>
+      <c r="E754" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F754" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G754" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H754" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I754" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J754" s="4" t="s">
+        <v>1988</v>
+      </c>
+      <c r="K754" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L754" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="755">
-      <c r="B755" s="2"/>
-      <c r="C755" s="3"/>
-      <c r="D755" s="1"/>
-      <c r="E755" s="1"/>
-      <c r="F755" s="1"/>
-      <c r="G755" s="1"/>
-      <c r="H755" s="1"/>
-      <c r="I755" s="1"/>
-      <c r="J755" s="1"/>
-      <c r="K755" s="1"/>
-      <c r="L755" s="1"/>
+      <c r="A755" s="1">
+        <v>754.0</v>
+      </c>
+      <c r="B755" s="2">
+        <v>45736.0</v>
+      </c>
+      <c r="C755" s="3" t="s">
+        <v>1989</v>
+      </c>
+      <c r="D755" s="1" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E755" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F755" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G755" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H755" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I755" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J755" s="4" t="s">
+        <v>1991</v>
+      </c>
+      <c r="K755" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L755" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="756">
       <c r="B756" s="2"/>
@@ -48265,7 +48537,15 @@
     <hyperlink r:id="rId744" ref="J745"/>
     <hyperlink r:id="rId745" ref="J746"/>
     <hyperlink r:id="rId746" ref="J747"/>
+    <hyperlink r:id="rId747" ref="J748"/>
+    <hyperlink r:id="rId748" ref="J749"/>
+    <hyperlink r:id="rId749" ref="J750"/>
+    <hyperlink r:id="rId750" ref="J751"/>
+    <hyperlink r:id="rId751" ref="J752"/>
+    <hyperlink r:id="rId752" ref="J753"/>
+    <hyperlink r:id="rId753" ref="J754"/>
+    <hyperlink r:id="rId754" ref="J755"/>
   </hyperlinks>
-  <drawing r:id="rId747"/>
+  <drawing r:id="rId755"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 1 new case
</commit_message>
<xml_diff>
--- a/tools/ExporterSheet.xlsx
+++ b/tools/ExporterSheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12332" uniqueCount="3151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12342" uniqueCount="3154">
   <si>
     <t>NOUMBER</t>
   </si>
@@ -9464,6 +9464,15 @@
   </si>
   <si>
     <t>https://u.to/4zkwIg</t>
+  </si>
+  <si>
+    <t>369787755229872130</t>
+  </si>
+  <si>
+    <t>mr.su.</t>
+  </si>
+  <si>
+    <t>https://u.to/JEMyIg</t>
   </si>
 </sst>
 </file>
@@ -56610,9 +56619,39 @@
       <c r="A1234" s="1">
         <v>1233.0</v>
       </c>
-      <c r="B1234" s="3"/>
-      <c r="C1234" s="2"/>
-      <c r="D1234" s="7"/>
+      <c r="B1234" s="3">
+        <v>45739.0</v>
+      </c>
+      <c r="C1234" s="2" t="s">
+        <v>3151</v>
+      </c>
+      <c r="D1234" s="2" t="s">
+        <v>3152</v>
+      </c>
+      <c r="E1234" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1234" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1234" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1234" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1234" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1234" s="4" t="s">
+        <v>3153</v>
+      </c>
+      <c r="K1234" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="L1234" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="1235">
       <c r="A1235" s="1">
@@ -65615,7 +65654,8 @@
     <hyperlink r:id="rId1085" ref="J1231"/>
     <hyperlink r:id="rId1086" ref="J1232"/>
     <hyperlink r:id="rId1087" ref="J1233"/>
+    <hyperlink r:id="rId1088" ref="J1234"/>
   </hyperlinks>
-  <drawing r:id="rId1088"/>
+  <drawing r:id="rId1089"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 2 new cases
</commit_message>
<xml_diff>
--- a/tools/ExporterSheet.xlsx
+++ b/tools/ExporterSheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14962" uniqueCount="3430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14984" uniqueCount="3436">
   <si>
     <t>NOUMBER</t>
   </si>
@@ -10301,6 +10301,24 @@
   </si>
   <si>
     <t>https://tinyurl.com/3s67dxdf</t>
+  </si>
+  <si>
+    <t>948244172358451210</t>
+  </si>
+  <si>
+    <t>.kerensky.</t>
+  </si>
+  <si>
+    <t>https://steam-ticket50.com/8320521963</t>
+  </si>
+  <si>
+    <t>976462371696545802</t>
+  </si>
+  <si>
+    <t>zelix099</t>
+  </si>
+  <si>
+    <t>https://t.me/+YtxFBk0f6Jw4NGMx</t>
   </si>
 </sst>
 </file>
@@ -66346,42 +66364,90 @@
         <v>23</v>
       </c>
       <c r="M1360" s="1" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
     </row>
     <row r="1361">
       <c r="A1361" s="1">
         <v>1360.0</v>
       </c>
-      <c r="B1361" s="2"/>
-      <c r="C1361" s="2"/>
-      <c r="D1361" s="3"/>
-      <c r="E1361" s="3"/>
-      <c r="F1361" s="1"/>
-      <c r="G1361" s="1"/>
-      <c r="H1361" s="1"/>
-      <c r="I1361" s="1"/>
-      <c r="J1361" s="1"/>
-      <c r="K1361" s="1"/>
-      <c r="L1361" s="1"/>
-      <c r="M1361" s="1"/>
+      <c r="B1361" s="2">
+        <v>45744.0</v>
+      </c>
+      <c r="C1361" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1361" s="3" t="s">
+        <v>3430</v>
+      </c>
+      <c r="E1361" s="3" t="s">
+        <v>3431</v>
+      </c>
+      <c r="F1361" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1361" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1361" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1361" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1361" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1361" s="4" t="s">
+        <v>3432</v>
+      </c>
+      <c r="L1361" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1361" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="1362">
       <c r="A1362" s="1">
         <v>1361.0</v>
       </c>
-      <c r="B1362" s="2"/>
-      <c r="C1362" s="2"/>
-      <c r="D1362" s="3"/>
-      <c r="E1362" s="3"/>
-      <c r="F1362" s="1"/>
-      <c r="G1362" s="1"/>
-      <c r="H1362" s="1"/>
-      <c r="I1362" s="1"/>
-      <c r="J1362" s="1"/>
-      <c r="K1362" s="1"/>
-      <c r="L1362" s="1"/>
-      <c r="M1362" s="1"/>
+      <c r="B1362" s="2">
+        <v>45744.0</v>
+      </c>
+      <c r="C1362" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D1362" s="3" t="s">
+        <v>3433</v>
+      </c>
+      <c r="E1362" s="3" t="s">
+        <v>3434</v>
+      </c>
+      <c r="F1362" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G1362" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H1362" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I1362" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J1362" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="K1362" s="4" t="s">
+        <v>3435</v>
+      </c>
+      <c r="L1362" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1362" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="1363">
       <c r="A1363" s="1">
@@ -73907,7 +73973,9 @@
     <hyperlink r:id="rId1094" ref="K1356"/>
     <hyperlink r:id="rId1095" ref="K1357"/>
     <hyperlink r:id="rId1096" ref="K1360"/>
+    <hyperlink r:id="rId1097" ref="K1361"/>
+    <hyperlink r:id="rId1098" ref="K1362"/>
   </hyperlinks>
-  <drawing r:id="rId1097"/>
+  <drawing r:id="rId1099"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 3 new cases
</commit_message>
<xml_diff>
--- a/tools/ExporterSheet.xlsx
+++ b/tools/ExporterSheet.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1373"/>
+  <dimension ref="A1:M1376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>https://discord.gg/pornhub</t>
+          <t>https://discord.gg/mAxhFjvARq</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
@@ -5427,7 +5427,7 @@
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>oak6073</t>
+          <t>deleted_user_52158dd9d758</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -5677,7 +5677,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>https://discord.gg/pornhub</t>
+          <t>https://discord.gg/mAxhFjvARq</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -5687,7 +5687,7 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>https://discord.gg/pornhub</t>
+          <t>https://discord.gg/mAxhFjvARq</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
@@ -5947,7 +5947,7 @@
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -8742,7 +8742,7 @@
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -9847,7 +9847,7 @@
       </c>
       <c r="M145" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -9912,7 +9912,7 @@
       </c>
       <c r="M146" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -10562,7 +10562,7 @@
       </c>
       <c r="M156" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="M159" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -11862,7 +11862,7 @@
       </c>
       <c r="M176" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -11927,7 +11927,7 @@
       </c>
       <c r="M177" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -12057,7 +12057,7 @@
       </c>
       <c r="M179" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -12252,7 +12252,7 @@
       </c>
       <c r="M182" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -12577,7 +12577,7 @@
       </c>
       <c r="M187" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -12642,7 +12642,7 @@
       </c>
       <c r="M188" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -12707,7 +12707,7 @@
       </c>
       <c r="M189" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -12772,7 +12772,7 @@
       </c>
       <c r="M190" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -12902,7 +12902,7 @@
       </c>
       <c r="M192" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -12967,7 +12967,7 @@
       </c>
       <c r="M193" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -16242,7 +16242,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>deleted_user_a8027b3745c</t>
+          <t>deleted_user_a8027b3745c1</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -18882,7 +18882,7 @@
       </c>
       <c r="M284" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -19102,7 +19102,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>minhduc10a7</t>
+          <t>mduc_2811</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -19987,7 +19987,7 @@
       </c>
       <c r="M301" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -21482,7 +21482,7 @@
       </c>
       <c r="M324" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -25382,7 +25382,7 @@
       </c>
       <c r="M384" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -29112,7 +29112,7 @@
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>seepy2</t>
+          <t>jap_flower</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -32727,7 +32727,7 @@
       </c>
       <c r="M497" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -33962,7 +33962,7 @@
       </c>
       <c r="M516" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -35847,7 +35847,7 @@
       </c>
       <c r="M545" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -37237,7 +37237,7 @@
       </c>
       <c r="E567" t="inlineStr">
         <is>
-          <t>slsasindu2</t>
+          <t>deleted_user_d3f08df5106a</t>
         </is>
       </c>
       <c r="F567" t="inlineStr">
@@ -38382,7 +38382,7 @@
       </c>
       <c r="M584" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -38447,7 +38447,7 @@
       </c>
       <c r="M585" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -38512,7 +38512,7 @@
       </c>
       <c r="M586" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -39487,7 +39487,7 @@
       </c>
       <c r="M601" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -41462,7 +41462,7 @@
       </c>
       <c r="E632" t="inlineStr">
         <is>
-          <t>dinnerbog5989</t>
+          <t>deleted_user_d5a2e5aa30bd</t>
         </is>
       </c>
       <c r="F632" t="inlineStr">
@@ -41592,7 +41592,7 @@
       </c>
       <c r="E634" t="inlineStr">
         <is>
-          <t>chris050499</t>
+          <t>deleted_user_07717c6c5862</t>
         </is>
       </c>
       <c r="F634" t="inlineStr">
@@ -42242,7 +42242,7 @@
       </c>
       <c r="E644" t="inlineStr">
         <is>
-          <t>zheax8905</t>
+          <t>deleted_user_d9e0bd040359</t>
         </is>
       </c>
       <c r="F644" t="inlineStr">
@@ -43192,7 +43192,7 @@
       </c>
       <c r="M658" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -43452,7 +43452,7 @@
       </c>
       <c r="M662" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -43517,7 +43517,7 @@
       </c>
       <c r="M663" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -44232,7 +44232,7 @@
       </c>
       <c r="M674" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -44297,7 +44297,7 @@
       </c>
       <c r="M675" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -44687,7 +44687,7 @@
       </c>
       <c r="M681" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -46377,7 +46377,7 @@
       </c>
       <c r="M707" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -46442,7 +46442,7 @@
       </c>
       <c r="M708" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -46962,7 +46962,7 @@
       </c>
       <c r="M716" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -47352,7 +47352,7 @@
       </c>
       <c r="M722" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -48132,7 +48132,7 @@
       </c>
       <c r="M734" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -48782,7 +48782,7 @@
       </c>
       <c r="M744" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -48847,7 +48847,7 @@
       </c>
       <c r="M745" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -48912,7 +48912,7 @@
       </c>
       <c r="M746" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -48977,7 +48977,7 @@
       </c>
       <c r="M747" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -50147,7 +50147,7 @@
       </c>
       <c r="M765" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -50537,7 +50537,7 @@
       </c>
       <c r="M771" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -51577,7 +51577,7 @@
       </c>
       <c r="M787" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -51967,7 +51967,7 @@
       </c>
       <c r="M793" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -52812,7 +52812,7 @@
       </c>
       <c r="M806" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -53982,7 +53982,7 @@
       </c>
       <c r="M824" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -57427,7 +57427,7 @@
       </c>
       <c r="M877" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -57557,7 +57557,7 @@
       </c>
       <c r="M879" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -60417,7 +60417,7 @@
       </c>
       <c r="M923" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -62302,7 +62302,7 @@
       </c>
       <c r="M952" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -63732,7 +63732,7 @@
       </c>
       <c r="M974" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -64967,7 +64967,7 @@
       </c>
       <c r="M993" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -66982,7 +66982,7 @@
       </c>
       <c r="M1024" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -67047,7 +67047,7 @@
       </c>
       <c r="M1025" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -67112,7 +67112,7 @@
       </c>
       <c r="M1026" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -67502,7 +67502,7 @@
       </c>
       <c r="M1032" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -67827,7 +67827,7 @@
       </c>
       <c r="M1037" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -68867,7 +68867,7 @@
       </c>
       <c r="M1053" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -72442,7 +72442,7 @@
       </c>
       <c r="M1108" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -72597,7 +72597,7 @@
       </c>
       <c r="E1111" t="inlineStr">
         <is>
-          <t>deleted_user_d54e66d45a1</t>
+          <t>deleted_user_d54e66d45a1f</t>
         </is>
       </c>
       <c r="F1111" t="inlineStr">
@@ -85532,7 +85532,7 @@
       </c>
       <c r="E1310" t="inlineStr">
         <is>
-          <t>laraxzx012</t>
+          <t>deleted_user_fba83ec9bd9d</t>
         </is>
       </c>
       <c r="F1310" t="inlineStr">
@@ -85767,7 +85767,7 @@
       </c>
       <c r="M1313" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -87027,7 +87027,7 @@
       </c>
       <c r="E1333" t="inlineStr">
         <is>
-          <t>litenetwork_official</t>
+          <t>deleted_user_00e9620d893e</t>
         </is>
       </c>
       <c r="F1333" t="inlineStr">
@@ -87327,7 +87327,7 @@
       </c>
       <c r="M1337" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -87457,7 +87457,7 @@
       </c>
       <c r="M1339" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -87522,7 +87522,7 @@
       </c>
       <c r="M1340" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -88107,7 +88107,7 @@
       </c>
       <c r="M1349" t="inlineStr">
         <is>
-          <t>INACTIVE</t>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>
@@ -88172,7 +88172,7 @@
       </c>
       <c r="M1350" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -88237,7 +88237,7 @@
       </c>
       <c r="M1351" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -88367,7 +88367,7 @@
       </c>
       <c r="M1353" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -88432,7 +88432,7 @@
       </c>
       <c r="M1354" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -88497,7 +88497,7 @@
       </c>
       <c r="M1355" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -88562,7 +88562,7 @@
       </c>
       <c r="M1356" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -88627,7 +88627,7 @@
       </c>
       <c r="M1357" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -88887,7 +88887,7 @@
       </c>
       <c r="M1361" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -88952,7 +88952,7 @@
       </c>
       <c r="M1362" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -89017,7 +89017,7 @@
       </c>
       <c r="M1363" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -89147,7 +89147,7 @@
       </c>
       <c r="M1365" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -89212,7 +89212,7 @@
       </c>
       <c r="M1366" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -89342,7 +89342,7 @@
       </c>
       <c r="M1368" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -89472,7 +89472,7 @@
       </c>
       <c r="M1370" t="inlineStr">
         <is>
-          <t>ACTIVE</t>
+          <t>INACTIVE</t>
         </is>
       </c>
     </row>
@@ -89668,6 +89668,201 @@
       <c r="M1373" t="inlineStr">
         <is>
           <t>UNKNOWN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1373</t>
+        </is>
+      </c>
+      <c r="B1374" s="1" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>PROJECT_CW</t>
+        </is>
+      </c>
+      <c r="D1374" t="inlineStr">
+        <is>
+          <t>812972922124763136</t>
+        </is>
+      </c>
+      <c r="E1374" t="inlineStr">
+        <is>
+          <t>quaresma007</t>
+        </is>
+      </c>
+      <c r="F1374" t="inlineStr">
+        <is>
+          <t>Automated Messaging Campaigns</t>
+        </is>
+      </c>
+      <c r="G1374" t="inlineStr">
+        <is>
+          <t>Phishing Website</t>
+        </is>
+      </c>
+      <c r="H1374" t="inlineStr">
+        <is>
+          <t>Cloned Steam Pages</t>
+        </is>
+      </c>
+      <c r="I1374" t="inlineStr">
+        <is>
+          <t>Steam Accounts</t>
+        </is>
+      </c>
+      <c r="J1374" t="inlineStr">
+        <is>
+          <t>Steam</t>
+        </is>
+      </c>
+      <c r="K1374" t="inlineStr">
+        <is>
+          <t>https://steamgiftcard.cfd/1053910953</t>
+        </is>
+      </c>
+      <c r="L1374" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="M1374" t="inlineStr">
+        <is>
+          <t>ACTIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1374</t>
+        </is>
+      </c>
+      <c r="B1375" s="1" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>PROJECT_CW</t>
+        </is>
+      </c>
+      <c r="D1375" t="inlineStr">
+        <is>
+          <t>1117625423325581472</t>
+        </is>
+      </c>
+      <c r="E1375" t="inlineStr">
+        <is>
+          <t>lilpooh47</t>
+        </is>
+      </c>
+      <c r="F1375" t="inlineStr">
+        <is>
+          <t>Automated Messaging Campaigns</t>
+        </is>
+      </c>
+      <c r="G1375" t="inlineStr">
+        <is>
+          <t>Phishing Website</t>
+        </is>
+      </c>
+      <c r="H1375" t="inlineStr">
+        <is>
+          <t>Cloned Steam Pages</t>
+        </is>
+      </c>
+      <c r="I1375" t="inlineStr">
+        <is>
+          <t>Steam Accounts</t>
+        </is>
+      </c>
+      <c r="J1375" t="inlineStr">
+        <is>
+          <t>Steam</t>
+        </is>
+      </c>
+      <c r="K1375" t="inlineStr">
+        <is>
+          <t>https://steamgiftcard.cfd/1053910953</t>
+        </is>
+      </c>
+      <c r="L1375" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="M1375" t="inlineStr">
+        <is>
+          <t>ACTIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1375</t>
+        </is>
+      </c>
+      <c r="B1376" s="1" t="n">
+        <v>45748</v>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>PROJECT_CW</t>
+        </is>
+      </c>
+      <c r="D1376" t="inlineStr">
+        <is>
+          <t>541980998569820160</t>
+        </is>
+      </c>
+      <c r="E1376" t="inlineStr">
+        <is>
+          <t>lucek6876</t>
+        </is>
+      </c>
+      <c r="F1376" t="inlineStr">
+        <is>
+          <t>Markdown URL Obfuscation</t>
+        </is>
+      </c>
+      <c r="G1376" t="inlineStr">
+        <is>
+          <t>Phishing Website</t>
+        </is>
+      </c>
+      <c r="H1376" t="inlineStr">
+        <is>
+          <t>Cloned Steam Pages</t>
+        </is>
+      </c>
+      <c r="I1376" t="inlineStr">
+        <is>
+          <t>Steam Accounts</t>
+        </is>
+      </c>
+      <c r="J1376" t="inlineStr">
+        <is>
+          <t>Steam</t>
+        </is>
+      </c>
+      <c r="K1376" t="inlineStr">
+        <is>
+          <t>https://tinyurl.com/296xr9aa</t>
+        </is>
+      </c>
+      <c r="L1376" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="M1376" t="inlineStr">
+        <is>
+          <t>ACTIVE</t>
         </is>
       </c>
     </row>

</xml_diff>